<commit_message>
add WB_16KHz speech files to the dataset, website documentation
</commit_message>
<xml_diff>
--- a/p835_reference_conditions/CSP835_Ref_Conditions.xlsx
+++ b/p835_reference_conditions/CSP835_Ref_Conditions.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\hitapp\P.835\p835_reference_conditions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E03D5BA-32C5-4122-867C-26DCC1784D0C}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{124793B3-9CD4-46FE-8351-961C460B0B9F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="12852" xr2:uid="{26D8FBFA-0696-4DB3-897E-8243390CDEAA}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="12852" activeTab="4" xr2:uid="{26D8FBFA-0696-4DB3-897E-8243390CDEAA}"/>
   </bookViews>
   <sheets>
     <sheet name="description" sheetId="2" r:id="rId1"/>
     <sheet name="testplan" sheetId="1" r:id="rId2"/>
-    <sheet name="results per file BAK" sheetId="3" r:id="rId3"/>
-    <sheet name="results per condition" sheetId="4" r:id="rId4"/>
-    <sheet name="plots" sheetId="5" r:id="rId5"/>
+    <sheet name="Fullband-results per file" sheetId="3" r:id="rId3"/>
+    <sheet name="Fullband-results per condition" sheetId="4" r:id="rId4"/>
+    <sheet name="Fullband-plots" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="243">
   <si>
     <t>c1</t>
   </si>
@@ -148,9 +148,6 @@
     <t>Num</t>
   </si>
   <si>
-    <t>BW</t>
-  </si>
-  <si>
     <t>Condition Name</t>
   </si>
   <si>
@@ -737,6 +734,30 @@
   </si>
   <si>
     <t>40/40</t>
+  </si>
+  <si>
+    <t>references</t>
+  </si>
+  <si>
+    <t>sample rate</t>
+  </si>
+  <si>
+    <t>48000Hz</t>
+  </si>
+  <si>
+    <t>audio bandwidth</t>
+  </si>
+  <si>
+    <t>16000Hz</t>
+  </si>
+  <si>
+    <t>WB</t>
+  </si>
+  <si>
+    <t>degraded_fullband_48KHz</t>
+  </si>
+  <si>
+    <t>degraded_WB_16KHz</t>
   </si>
 </sst>
 </file>
@@ -798,7 +819,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -817,6 +838,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -918,7 +942,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>plots!$C$22</c:f>
+              <c:f>'Fullband-plots'!$C$22</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -951,9 +975,76 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'Fullband-plots'!$F$23:$F$27</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="5"/>
+                  <c:pt idx="0">
+                    <c:v>0.29399999999999998</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.324756660834989</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.30430944003451099</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.22306152136773999</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.122812955386261</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'Fullband-plots'!$F$23:$F$27</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="5"/>
+                  <c:pt idx="0">
+                    <c:v>0.29399999999999998</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.324756660834989</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.30430944003451099</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.22306152136773999</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.122812955386261</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:cat>
             <c:numRef>
-              <c:f>plots!$A$23:$A$27</c:f>
+              <c:f>'Fullband-plots'!$A$23:$A$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -977,7 +1068,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>plots!$C$23:$C$27</c:f>
+              <c:f>'Fullband-plots'!$C$23:$C$27</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1011,7 +1102,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>plots!$B$22</c:f>
+              <c:f>'Fullband-plots'!$B$22</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1044,9 +1135,76 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'Fullband-plots'!$E$23:$E$27</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="5"/>
+                  <c:pt idx="0">
+                    <c:v>0.42333568543663103</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.39027640108581602</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.32426568627302699</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.27187430871537299</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.209743051210836</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'Fullband-plots'!$E$23:$E$27</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="5"/>
+                  <c:pt idx="0">
+                    <c:v>0.42333568543663103</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.39027640108581602</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.32426568627302699</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.27187430871537299</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.209743051210836</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:cat>
             <c:numRef>
-              <c:f>plots!$A$23:$A$27</c:f>
+              <c:f>'Fullband-plots'!$A$23:$A$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1070,7 +1228,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>plots!$B$23:$B$27</c:f>
+              <c:f>'Fullband-plots'!$B$23:$B$27</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1104,7 +1262,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>plots!$D$22</c:f>
+              <c:f>'Fullband-plots'!$D$22</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1137,9 +1295,76 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'Fullband-plots'!$G$23:$G$27</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="5"/>
+                  <c:pt idx="0">
+                    <c:v>0.267695004407283</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.268942273472282</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.317074865904308</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.23268538219111001</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.20755246321142001</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'Fullband-plots'!$G$23:$G$27</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="5"/>
+                  <c:pt idx="0">
+                    <c:v>0.267695004407283</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.268942273472282</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.317074865904308</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.23268538219111001</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.20755246321142001</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:cat>
             <c:numRef>
-              <c:f>plots!$A$23:$A$27</c:f>
+              <c:f>'Fullband-plots'!$A$23:$A$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1163,7 +1388,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>plots!$D$23:$D$27</c:f>
+              <c:f>'Fullband-plots'!$D$23:$D$27</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1593,7 +1818,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>plots!$C$42</c:f>
+              <c:f>'Fullband-plots'!$C$42</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1626,9 +1851,76 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'Fullband-plots'!$F$43:$F$47</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="5"/>
+                  <c:pt idx="0">
+                    <c:v>0.413998141950494</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.29440044472695198</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.31476409685850598</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.262117413503068</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.122812955386261</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'Fullband-plots'!$F$43:$F$47</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="5"/>
+                  <c:pt idx="0">
+                    <c:v>0.413998141950494</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.29440044472695198</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.31476409685850598</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.262117413503068</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.122812955386261</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:cat>
             <c:numRef>
-              <c:f>plots!$A$43:$A$47</c:f>
+              <c:f>'Fullband-plots'!$A$43:$A$47</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1652,7 +1944,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>plots!$C$43:$C$47</c:f>
+              <c:f>'Fullband-plots'!$C$43:$C$47</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1686,7 +1978,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>plots!$B$42</c:f>
+              <c:f>'Fullband-plots'!$B$42</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1719,9 +2011,76 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'Fullband-plots'!$E$43:$E$47</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="5"/>
+                  <c:pt idx="0">
+                    <c:v>0.28764935919649398</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.36350287997334801</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.28140240761331597</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.25677841390224698</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.209743051210836</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'Fullband-plots'!$E$43:$E$47</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="5"/>
+                  <c:pt idx="0">
+                    <c:v>0.28764935919649398</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.36350287997334801</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.28140240761331597</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.25677841390224698</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.209743051210836</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:cat>
             <c:numRef>
-              <c:f>plots!$A$43:$A$47</c:f>
+              <c:f>'Fullband-plots'!$A$43:$A$47</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1745,7 +2104,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>plots!$B$43:$B$47</c:f>
+              <c:f>'Fullband-plots'!$B$43:$B$47</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1779,7 +2138,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>plots!$D$42</c:f>
+              <c:f>'Fullband-plots'!$D$42</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1812,9 +2171,76 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'Fullband-plots'!$G$43:$G$47</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="5"/>
+                  <c:pt idx="0">
+                    <c:v>0.28235706617776102</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.32097079291555602</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.26230585747858598</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.206850311293097</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.20755246321142001</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'Fullband-plots'!$G$43:$G$47</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="5"/>
+                  <c:pt idx="0">
+                    <c:v>0.28235706617776102</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.32097079291555602</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.26230585747858598</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.206850311293097</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.20755246321142001</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:cat>
             <c:numRef>
-              <c:f>plots!$A$43:$A$47</c:f>
+              <c:f>'Fullband-plots'!$A$43:$A$47</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1838,7 +2264,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>plots!$D$43:$D$47</c:f>
+              <c:f>'Fullband-plots'!$D$43:$D$47</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="5"/>
@@ -2264,7 +2690,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>plots!$C$58</c:f>
+              <c:f>'Fullband-plots'!$C$58</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2297,9 +2723,70 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'Fullband-plots'!$F$59:$F$62</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>0.35469556125848301</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.34413677171592499</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.30743382305067701</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.122812955386261</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'Fullband-plots'!$F$59:$F$62</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>0.35469556125848301</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.34413677171592499</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.30743382305067701</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.122812955386261</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>plots!$A$59:$A$62</c:f>
+              <c:f>'Fullband-plots'!$A$59:$A$62</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -2319,7 +2806,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>plots!$C$59:$C$62</c:f>
+              <c:f>'Fullband-plots'!$C$59:$C$62</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="4"/>
@@ -2350,7 +2837,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>plots!$B$58</c:f>
+              <c:f>'Fullband-plots'!$B$58</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2383,9 +2870,70 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'Fullband-plots'!$E$59:$E$62</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>0.37810673874231898</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.28392542517151098</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.29217954905997201</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.209743051210836</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'Fullband-plots'!$E$59:$E$62</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>0.37810673874231898</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.28392542517151098</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.29217954905997201</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.209743051210836</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>plots!$A$59:$A$62</c:f>
+              <c:f>'Fullband-plots'!$A$59:$A$62</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -2405,7 +2953,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>plots!$B$59:$B$62</c:f>
+              <c:f>'Fullband-plots'!$B$59:$B$62</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="4"/>
@@ -2436,7 +2984,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>plots!$D$58</c:f>
+              <c:f>'Fullband-plots'!$D$58</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2469,9 +3017,70 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'Fullband-plots'!$G$59:$G$62</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>0.295076460679361</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.256624238917527</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.26223917082703202</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.20755246321142001</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'Fullband-plots'!$G$59:$G$62</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>0.295076460679361</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.256624238917527</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.26223917082703202</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.20755246321142001</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>plots!$A$59:$A$62</c:f>
+              <c:f>'Fullband-plots'!$A$59:$A$62</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -2491,7 +3100,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>plots!$D$59:$D$62</c:f>
+              <c:f>'Fullband-plots'!$D$59:$D$62</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="4"/>
@@ -4466,14 +5075,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>259080</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>15240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
       <xdr:row>35</xdr:row>
       <xdr:rowOff>144780</xdr:rowOff>
     </xdr:to>
@@ -4502,16 +5111,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>236220</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>434340</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>83820</xdr:rowOff>
+      <xdr:rowOff>121920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>53340</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>320040</xdr:colOff>
       <xdr:row>57</xdr:row>
-      <xdr:rowOff>60960</xdr:rowOff>
+      <xdr:rowOff>99060</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4538,16 +5147,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>289560</xdr:colOff>
-      <xdr:row>59</xdr:row>
-      <xdr:rowOff>99060</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>426720</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>121920</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>327660</xdr:colOff>
       <xdr:row>79</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:rowOff>167640</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4872,10 +5481,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EF8797D-78C9-4C44-9CB3-1E03D4B2359C}">
-  <dimension ref="A1:C32"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4945,7 +5554,7 @@
         <v>19</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -4953,7 +5562,7 @@
         <v>20</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -4969,7 +5578,7 @@
         <v>35</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -4977,7 +5586,7 @@
         <v>23</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -4993,16 +5602,16 @@
         <v>25</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B17" s="2"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -5010,7 +5619,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>29</v>
       </c>
@@ -5018,13 +5627,65 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>235</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C32" s="7"/>
+        <v>241</v>
+      </c>
+      <c r="B21" s="2"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="10" t="s">
+        <v>236</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="10" t="s">
+        <v>238</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>242</v>
+      </c>
+      <c r="B24" s="2"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="10" t="s">
+        <v>236</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="10" t="s">
+        <v>238</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C33" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5033,259 +5694,302 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2660FF2D-5F2E-448E-A792-FA8B96D7B497}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B14"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>38</v>
       </c>
       <c r="B1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" t="s">
         <v>40</v>
-      </c>
-      <c r="C1" t="s">
-        <v>39</v>
       </c>
       <c r="D1" t="s">
         <v>41</v>
       </c>
       <c r="E1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+        <v>241</v>
+      </c>
+      <c r="F1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="C2" t="s">
-        <v>215</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="E2" s="10"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D2" s="11"/>
+      <c r="E2" t="s">
+        <v>214</v>
+      </c>
+      <c r="F2" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
       </c>
-      <c r="C3" t="s">
-        <v>215</v>
+      <c r="C3">
+        <v>40</v>
       </c>
       <c r="D3">
-        <v>40</v>
-      </c>
-      <c r="E3">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E3" t="s">
+        <v>214</v>
+      </c>
+      <c r="F3" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
       </c>
-      <c r="C4" t="s">
-        <v>215</v>
+      <c r="C4">
+        <v>40</v>
       </c>
       <c r="D4">
-        <v>40</v>
-      </c>
-      <c r="E4">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E4" t="s">
+        <v>214</v>
+      </c>
+      <c r="F4" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>2</v>
       </c>
-      <c r="C5" t="s">
-        <v>215</v>
+      <c r="C5">
+        <v>40</v>
       </c>
       <c r="D5">
-        <v>40</v>
-      </c>
-      <c r="E5">
         <v>24</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E5" t="s">
+        <v>214</v>
+      </c>
+      <c r="F5" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>3</v>
       </c>
-      <c r="C6" t="s">
-        <v>215</v>
+      <c r="C6">
+        <v>40</v>
       </c>
       <c r="D6">
-        <v>40</v>
-      </c>
-      <c r="E6">
         <v>32</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E6" t="s">
+        <v>214</v>
+      </c>
+      <c r="F6" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>4</v>
       </c>
-      <c r="C7" t="s">
-        <v>215</v>
+      <c r="C7">
+        <v>40</v>
       </c>
       <c r="D7">
         <v>40</v>
       </c>
-      <c r="E7">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E7" t="s">
+        <v>214</v>
+      </c>
+      <c r="F7" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
       </c>
-      <c r="C8" t="s">
-        <v>215</v>
+      <c r="C8">
+        <v>0</v>
       </c>
       <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
         <v>40</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E8" t="s">
+        <v>214</v>
+      </c>
+      <c r="F8" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
       </c>
-      <c r="C9" t="s">
-        <v>215</v>
+      <c r="C9">
+        <v>10</v>
       </c>
       <c r="D9">
-        <v>10</v>
-      </c>
-      <c r="E9">
         <v>40</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E9" t="s">
+        <v>214</v>
+      </c>
+      <c r="F9" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>7</v>
       </c>
-      <c r="C10" t="s">
-        <v>215</v>
+      <c r="C10">
+        <v>20</v>
       </c>
       <c r="D10">
-        <v>20</v>
-      </c>
-      <c r="E10">
         <v>40</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E10" t="s">
+        <v>214</v>
+      </c>
+      <c r="F10" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>8</v>
       </c>
-      <c r="C11" t="s">
-        <v>215</v>
+      <c r="C11">
+        <v>30</v>
       </c>
       <c r="D11">
-        <v>30</v>
-      </c>
-      <c r="E11">
         <v>40</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E11" t="s">
+        <v>214</v>
+      </c>
+      <c r="F11" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
         <v>9</v>
       </c>
-      <c r="C12" t="s">
-        <v>215</v>
+      <c r="C12">
+        <v>10</v>
       </c>
       <c r="D12">
-        <v>10</v>
-      </c>
-      <c r="E12">
         <v>16</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E12" t="s">
+        <v>214</v>
+      </c>
+      <c r="F12" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
       </c>
-      <c r="C13" t="s">
-        <v>215</v>
+      <c r="C13">
+        <v>20</v>
       </c>
       <c r="D13">
-        <v>20</v>
-      </c>
-      <c r="E13">
         <v>24</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E13" t="s">
+        <v>214</v>
+      </c>
+      <c r="F13" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
         <v>11</v>
       </c>
-      <c r="C14" t="s">
-        <v>215</v>
+      <c r="C14">
+        <v>30</v>
       </c>
       <c r="D14">
-        <v>30</v>
-      </c>
-      <c r="E14">
         <v>32</v>
+      </c>
+      <c r="E14" t="s">
+        <v>214</v>
+      </c>
+      <c r="F14" t="s">
+        <v>240</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="C2:D2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5295,8 +5999,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9581DE09-F9A5-41EB-B924-712A6D38D56A}">
   <dimension ref="A1:M79"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D79"/>
+    <sheetView topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="D74" sqref="D74:D79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5315,51 +6019,51 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>51</v>
-      </c>
       <c r="D1" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="K1" s="6" t="s">
         <v>208</v>
       </c>
-      <c r="E1" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>212</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>213</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="K1" s="6" t="s">
+      <c r="L1" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>210</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" t="s">
         <v>52</v>
-      </c>
-      <c r="B2" t="s">
-        <v>53</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -5397,10 +6101,10 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" t="s">
         <v>54</v>
-      </c>
-      <c r="B3" t="s">
-        <v>55</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -5438,10 +6142,10 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" t="s">
         <v>56</v>
-      </c>
-      <c r="B4" t="s">
-        <v>57</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -5479,10 +6183,10 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" t="s">
         <v>58</v>
-      </c>
-      <c r="B5" t="s">
-        <v>59</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -5520,10 +6224,10 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6" t="s">
         <v>60</v>
-      </c>
-      <c r="B6" t="s">
-        <v>61</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -5561,10 +6265,10 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" t="s">
         <v>62</v>
-      </c>
-      <c r="B7" t="s">
-        <v>63</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -5602,10 +6306,10 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B8" t="s">
         <v>64</v>
-      </c>
-      <c r="B8" t="s">
-        <v>65</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -5643,10 +6347,10 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B9" t="s">
         <v>66</v>
-      </c>
-      <c r="B9" t="s">
-        <v>67</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -5684,10 +6388,10 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B10" t="s">
         <v>68</v>
-      </c>
-      <c r="B10" t="s">
-        <v>69</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -5725,10 +6429,10 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>69</v>
+      </c>
+      <c r="B11" t="s">
         <v>70</v>
-      </c>
-      <c r="B11" t="s">
-        <v>71</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -5766,10 +6470,10 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>71</v>
+      </c>
+      <c r="B12" t="s">
         <v>72</v>
-      </c>
-      <c r="B12" t="s">
-        <v>73</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -5807,10 +6511,10 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>73</v>
+      </c>
+      <c r="B13" t="s">
         <v>74</v>
-      </c>
-      <c r="B13" t="s">
-        <v>75</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -5848,10 +6552,10 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>111</v>
+      </c>
+      <c r="B14" t="s">
         <v>112</v>
-      </c>
-      <c r="B14" t="s">
-        <v>113</v>
       </c>
       <c r="C14">
         <v>2</v>
@@ -5889,10 +6593,10 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>113</v>
+      </c>
+      <c r="B15" t="s">
         <v>114</v>
-      </c>
-      <c r="B15" t="s">
-        <v>115</v>
       </c>
       <c r="C15">
         <v>2</v>
@@ -5930,10 +6634,10 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>115</v>
+      </c>
+      <c r="B16" t="s">
         <v>116</v>
-      </c>
-      <c r="B16" t="s">
-        <v>117</v>
       </c>
       <c r="C16">
         <v>2</v>
@@ -5971,10 +6675,10 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>117</v>
+      </c>
+      <c r="B17" t="s">
         <v>118</v>
-      </c>
-      <c r="B17" t="s">
-        <v>119</v>
       </c>
       <c r="C17">
         <v>2</v>
@@ -6012,10 +6716,10 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>119</v>
+      </c>
+      <c r="B18" t="s">
         <v>120</v>
-      </c>
-      <c r="B18" t="s">
-        <v>121</v>
       </c>
       <c r="C18">
         <v>2</v>
@@ -6053,10 +6757,10 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>121</v>
+      </c>
+      <c r="B19" t="s">
         <v>122</v>
-      </c>
-      <c r="B19" t="s">
-        <v>123</v>
       </c>
       <c r="C19">
         <v>2</v>
@@ -6094,10 +6798,10 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>123</v>
+      </c>
+      <c r="B20" t="s">
         <v>124</v>
-      </c>
-      <c r="B20" t="s">
-        <v>125</v>
       </c>
       <c r="C20">
         <v>3</v>
@@ -6135,10 +6839,10 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
+        <v>125</v>
+      </c>
+      <c r="B21" t="s">
         <v>126</v>
-      </c>
-      <c r="B21" t="s">
-        <v>127</v>
       </c>
       <c r="C21">
         <v>3</v>
@@ -6176,10 +6880,10 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
+        <v>127</v>
+      </c>
+      <c r="B22" t="s">
         <v>128</v>
-      </c>
-      <c r="B22" t="s">
-        <v>129</v>
       </c>
       <c r="C22">
         <v>3</v>
@@ -6217,10 +6921,10 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
+        <v>129</v>
+      </c>
+      <c r="B23" t="s">
         <v>130</v>
-      </c>
-      <c r="B23" t="s">
-        <v>131</v>
       </c>
       <c r="C23">
         <v>3</v>
@@ -6258,10 +6962,10 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
+        <v>131</v>
+      </c>
+      <c r="B24" t="s">
         <v>132</v>
-      </c>
-      <c r="B24" t="s">
-        <v>133</v>
       </c>
       <c r="C24">
         <v>3</v>
@@ -6299,10 +7003,10 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
+        <v>133</v>
+      </c>
+      <c r="B25" t="s">
         <v>134</v>
-      </c>
-      <c r="B25" t="s">
-        <v>135</v>
       </c>
       <c r="C25">
         <v>3</v>
@@ -6340,10 +7044,10 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
+        <v>135</v>
+      </c>
+      <c r="B26" t="s">
         <v>136</v>
-      </c>
-      <c r="B26" t="s">
-        <v>137</v>
       </c>
       <c r="C26">
         <v>4</v>
@@ -6381,10 +7085,10 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
+        <v>137</v>
+      </c>
+      <c r="B27" t="s">
         <v>138</v>
-      </c>
-      <c r="B27" t="s">
-        <v>139</v>
       </c>
       <c r="C27">
         <v>4</v>
@@ -6422,10 +7126,10 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
+        <v>139</v>
+      </c>
+      <c r="B28" t="s">
         <v>140</v>
-      </c>
-      <c r="B28" t="s">
-        <v>141</v>
       </c>
       <c r="C28">
         <v>4</v>
@@ -6463,10 +7167,10 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
+        <v>141</v>
+      </c>
+      <c r="B29" t="s">
         <v>142</v>
-      </c>
-      <c r="B29" t="s">
-        <v>143</v>
       </c>
       <c r="C29">
         <v>4</v>
@@ -6504,10 +7208,10 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
+        <v>143</v>
+      </c>
+      <c r="B30" t="s">
         <v>144</v>
-      </c>
-      <c r="B30" t="s">
-        <v>145</v>
       </c>
       <c r="C30">
         <v>4</v>
@@ -6545,10 +7249,10 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
+        <v>145</v>
+      </c>
+      <c r="B31" t="s">
         <v>146</v>
-      </c>
-      <c r="B31" t="s">
-        <v>147</v>
       </c>
       <c r="C31">
         <v>4</v>
@@ -6586,10 +7290,10 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
+        <v>147</v>
+      </c>
+      <c r="B32" t="s">
         <v>148</v>
-      </c>
-      <c r="B32" t="s">
-        <v>149</v>
       </c>
       <c r="C32">
         <v>5</v>
@@ -6627,10 +7331,10 @@
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
+        <v>149</v>
+      </c>
+      <c r="B33" t="s">
         <v>150</v>
-      </c>
-      <c r="B33" t="s">
-        <v>151</v>
       </c>
       <c r="C33">
         <v>5</v>
@@ -6668,10 +7372,10 @@
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
+        <v>151</v>
+      </c>
+      <c r="B34" t="s">
         <v>152</v>
-      </c>
-      <c r="B34" t="s">
-        <v>153</v>
       </c>
       <c r="C34">
         <v>5</v>
@@ -6709,10 +7413,10 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
+        <v>153</v>
+      </c>
+      <c r="B35" t="s">
         <v>154</v>
-      </c>
-      <c r="B35" t="s">
-        <v>155</v>
       </c>
       <c r="C35">
         <v>5</v>
@@ -6750,10 +7454,10 @@
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
+        <v>155</v>
+      </c>
+      <c r="B36" t="s">
         <v>156</v>
-      </c>
-      <c r="B36" t="s">
-        <v>157</v>
       </c>
       <c r="C36">
         <v>5</v>
@@ -6791,10 +7495,10 @@
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
+        <v>157</v>
+      </c>
+      <c r="B37" t="s">
         <v>158</v>
-      </c>
-      <c r="B37" t="s">
-        <v>159</v>
       </c>
       <c r="C37">
         <v>5</v>
@@ -6832,10 +7536,10 @@
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
+        <v>159</v>
+      </c>
+      <c r="B38" t="s">
         <v>160</v>
-      </c>
-      <c r="B38" t="s">
-        <v>161</v>
       </c>
       <c r="C38">
         <v>6</v>
@@ -6873,10 +7577,10 @@
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
+        <v>161</v>
+      </c>
+      <c r="B39" t="s">
         <v>162</v>
-      </c>
-      <c r="B39" t="s">
-        <v>163</v>
       </c>
       <c r="C39">
         <v>6</v>
@@ -6914,10 +7618,10 @@
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
+        <v>163</v>
+      </c>
+      <c r="B40" t="s">
         <v>164</v>
-      </c>
-      <c r="B40" t="s">
-        <v>165</v>
       </c>
       <c r="C40">
         <v>6</v>
@@ -6955,10 +7659,10 @@
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
+        <v>165</v>
+      </c>
+      <c r="B41" t="s">
         <v>166</v>
-      </c>
-      <c r="B41" t="s">
-        <v>167</v>
       </c>
       <c r="C41">
         <v>6</v>
@@ -6996,10 +7700,10 @@
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
+        <v>167</v>
+      </c>
+      <c r="B42" t="s">
         <v>168</v>
-      </c>
-      <c r="B42" t="s">
-        <v>169</v>
       </c>
       <c r="C42">
         <v>6</v>
@@ -7037,10 +7741,10 @@
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
+        <v>169</v>
+      </c>
+      <c r="B43" t="s">
         <v>170</v>
-      </c>
-      <c r="B43" t="s">
-        <v>171</v>
       </c>
       <c r="C43">
         <v>6</v>
@@ -7078,10 +7782,10 @@
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
+        <v>171</v>
+      </c>
+      <c r="B44" t="s">
         <v>172</v>
-      </c>
-      <c r="B44" t="s">
-        <v>173</v>
       </c>
       <c r="C44">
         <v>7</v>
@@ -7119,10 +7823,10 @@
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
+        <v>173</v>
+      </c>
+      <c r="B45" t="s">
         <v>174</v>
-      </c>
-      <c r="B45" t="s">
-        <v>175</v>
       </c>
       <c r="C45">
         <v>7</v>
@@ -7160,10 +7864,10 @@
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
+        <v>175</v>
+      </c>
+      <c r="B46" t="s">
         <v>176</v>
-      </c>
-      <c r="B46" t="s">
-        <v>177</v>
       </c>
       <c r="C46">
         <v>7</v>
@@ -7201,10 +7905,10 @@
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
+        <v>177</v>
+      </c>
+      <c r="B47" t="s">
         <v>178</v>
-      </c>
-      <c r="B47" t="s">
-        <v>179</v>
       </c>
       <c r="C47">
         <v>7</v>
@@ -7242,10 +7946,10 @@
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
+        <v>179</v>
+      </c>
+      <c r="B48" t="s">
         <v>180</v>
-      </c>
-      <c r="B48" t="s">
-        <v>181</v>
       </c>
       <c r="C48">
         <v>7</v>
@@ -7283,10 +7987,10 @@
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
+        <v>181</v>
+      </c>
+      <c r="B49" t="s">
         <v>182</v>
-      </c>
-      <c r="B49" t="s">
-        <v>183</v>
       </c>
       <c r="C49">
         <v>7</v>
@@ -7324,10 +8028,10 @@
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
+        <v>183</v>
+      </c>
+      <c r="B50" t="s">
         <v>184</v>
-      </c>
-      <c r="B50" t="s">
-        <v>185</v>
       </c>
       <c r="C50">
         <v>8</v>
@@ -7365,10 +8069,10 @@
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
+        <v>185</v>
+      </c>
+      <c r="B51" t="s">
         <v>186</v>
-      </c>
-      <c r="B51" t="s">
-        <v>187</v>
       </c>
       <c r="C51">
         <v>8</v>
@@ -7406,10 +8110,10 @@
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
+        <v>187</v>
+      </c>
+      <c r="B52" t="s">
         <v>188</v>
-      </c>
-      <c r="B52" t="s">
-        <v>189</v>
       </c>
       <c r="C52">
         <v>8</v>
@@ -7447,10 +8151,10 @@
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
+        <v>189</v>
+      </c>
+      <c r="B53" t="s">
         <v>190</v>
-      </c>
-      <c r="B53" t="s">
-        <v>191</v>
       </c>
       <c r="C53">
         <v>8</v>
@@ -7488,10 +8192,10 @@
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
+        <v>191</v>
+      </c>
+      <c r="B54" t="s">
         <v>192</v>
-      </c>
-      <c r="B54" t="s">
-        <v>193</v>
       </c>
       <c r="C54">
         <v>8</v>
@@ -7529,10 +8233,10 @@
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
+        <v>193</v>
+      </c>
+      <c r="B55" t="s">
         <v>194</v>
-      </c>
-      <c r="B55" t="s">
-        <v>195</v>
       </c>
       <c r="C55">
         <v>8</v>
@@ -7570,10 +8274,10 @@
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
+        <v>195</v>
+      </c>
+      <c r="B56" t="s">
         <v>196</v>
-      </c>
-      <c r="B56" t="s">
-        <v>197</v>
       </c>
       <c r="C56">
         <v>9</v>
@@ -7611,10 +8315,10 @@
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
+        <v>197</v>
+      </c>
+      <c r="B57" t="s">
         <v>198</v>
-      </c>
-      <c r="B57" t="s">
-        <v>199</v>
       </c>
       <c r="C57">
         <v>9</v>
@@ -7652,10 +8356,10 @@
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
+        <v>199</v>
+      </c>
+      <c r="B58" t="s">
         <v>200</v>
-      </c>
-      <c r="B58" t="s">
-        <v>201</v>
       </c>
       <c r="C58">
         <v>9</v>
@@ -7693,10 +8397,10 @@
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
+        <v>201</v>
+      </c>
+      <c r="B59" t="s">
         <v>202</v>
-      </c>
-      <c r="B59" t="s">
-        <v>203</v>
       </c>
       <c r="C59">
         <v>9</v>
@@ -7734,10 +8438,10 @@
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
+        <v>203</v>
+      </c>
+      <c r="B60" t="s">
         <v>204</v>
-      </c>
-      <c r="B60" t="s">
-        <v>205</v>
       </c>
       <c r="C60">
         <v>9</v>
@@ -7775,10 +8479,10 @@
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
+        <v>205</v>
+      </c>
+      <c r="B61" t="s">
         <v>206</v>
-      </c>
-      <c r="B61" t="s">
-        <v>207</v>
       </c>
       <c r="C61">
         <v>9</v>
@@ -7816,10 +8520,10 @@
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
+        <v>75</v>
+      </c>
+      <c r="B62" t="s">
         <v>76</v>
-      </c>
-      <c r="B62" t="s">
-        <v>77</v>
       </c>
       <c r="C62">
         <v>10</v>
@@ -7857,10 +8561,10 @@
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
+        <v>77</v>
+      </c>
+      <c r="B63" t="s">
         <v>78</v>
-      </c>
-      <c r="B63" t="s">
-        <v>79</v>
       </c>
       <c r="C63">
         <v>10</v>
@@ -7898,10 +8602,10 @@
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
+        <v>79</v>
+      </c>
+      <c r="B64" t="s">
         <v>80</v>
-      </c>
-      <c r="B64" t="s">
-        <v>81</v>
       </c>
       <c r="C64">
         <v>10</v>
@@ -7939,10 +8643,10 @@
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
+        <v>81</v>
+      </c>
+      <c r="B65" t="s">
         <v>82</v>
-      </c>
-      <c r="B65" t="s">
-        <v>83</v>
       </c>
       <c r="C65">
         <v>10</v>
@@ -7980,10 +8684,10 @@
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
+        <v>83</v>
+      </c>
+      <c r="B66" t="s">
         <v>84</v>
-      </c>
-      <c r="B66" t="s">
-        <v>85</v>
       </c>
       <c r="C66">
         <v>10</v>
@@ -8021,10 +8725,10 @@
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
+        <v>85</v>
+      </c>
+      <c r="B67" t="s">
         <v>86</v>
-      </c>
-      <c r="B67" t="s">
-        <v>87</v>
       </c>
       <c r="C67">
         <v>10</v>
@@ -8062,10 +8766,10 @@
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
+        <v>87</v>
+      </c>
+      <c r="B68" t="s">
         <v>88</v>
-      </c>
-      <c r="B68" t="s">
-        <v>89</v>
       </c>
       <c r="C68">
         <v>11</v>
@@ -8103,10 +8807,10 @@
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
+        <v>89</v>
+      </c>
+      <c r="B69" t="s">
         <v>90</v>
-      </c>
-      <c r="B69" t="s">
-        <v>91</v>
       </c>
       <c r="C69">
         <v>11</v>
@@ -8144,10 +8848,10 @@
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
+        <v>91</v>
+      </c>
+      <c r="B70" t="s">
         <v>92</v>
-      </c>
-      <c r="B70" t="s">
-        <v>93</v>
       </c>
       <c r="C70">
         <v>11</v>
@@ -8185,10 +8889,10 @@
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
+        <v>93</v>
+      </c>
+      <c r="B71" t="s">
         <v>94</v>
-      </c>
-      <c r="B71" t="s">
-        <v>95</v>
       </c>
       <c r="C71">
         <v>11</v>
@@ -8226,10 +8930,10 @@
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
+        <v>95</v>
+      </c>
+      <c r="B72" t="s">
         <v>96</v>
-      </c>
-      <c r="B72" t="s">
-        <v>97</v>
       </c>
       <c r="C72">
         <v>11</v>
@@ -8267,10 +8971,10 @@
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
+        <v>97</v>
+      </c>
+      <c r="B73" t="s">
         <v>98</v>
-      </c>
-      <c r="B73" t="s">
-        <v>99</v>
       </c>
       <c r="C73">
         <v>11</v>
@@ -8308,10 +9012,10 @@
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
+        <v>99</v>
+      </c>
+      <c r="B74" t="s">
         <v>100</v>
-      </c>
-      <c r="B74" t="s">
-        <v>101</v>
       </c>
       <c r="C74">
         <v>12</v>
@@ -8349,10 +9053,10 @@
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
+        <v>101</v>
+      </c>
+      <c r="B75" t="s">
         <v>102</v>
-      </c>
-      <c r="B75" t="s">
-        <v>103</v>
       </c>
       <c r="C75">
         <v>12</v>
@@ -8390,10 +9094,10 @@
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
+        <v>103</v>
+      </c>
+      <c r="B76" t="s">
         <v>104</v>
-      </c>
-      <c r="B76" t="s">
-        <v>105</v>
       </c>
       <c r="C76">
         <v>12</v>
@@ -8431,10 +9135,10 @@
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
+        <v>105</v>
+      </c>
+      <c r="B77" t="s">
         <v>106</v>
-      </c>
-      <c r="B77" t="s">
-        <v>107</v>
       </c>
       <c r="C77">
         <v>12</v>
@@ -8472,10 +9176,10 @@
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
+        <v>107</v>
+      </c>
+      <c r="B78" t="s">
         <v>108</v>
-      </c>
-      <c r="B78" t="s">
-        <v>109</v>
       </c>
       <c r="C78">
         <v>12</v>
@@ -8513,10 +9217,10 @@
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
+        <v>109</v>
+      </c>
+      <c r="B79" t="s">
         <v>110</v>
-      </c>
-      <c r="B79" t="s">
-        <v>111</v>
       </c>
       <c r="C79">
         <v>12</v>
@@ -8582,53 +9286,53 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" t="s">
         <v>40</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>41</v>
       </c>
-      <c r="C1" t="s">
-        <v>42</v>
-      </c>
       <c r="D1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" t="s">
         <v>46</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
+        <v>211</v>
+      </c>
+      <c r="G1" t="s">
+        <v>208</v>
+      </c>
+      <c r="H1" t="s">
         <v>47</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>212</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>209</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>48</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>213</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>210</v>
-      </c>
-      <c r="K1" t="s">
-        <v>49</v>
-      </c>
-      <c r="L1" t="s">
-        <v>214</v>
-      </c>
-      <c r="M1" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="B2" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="C2" s="10"/>
+      <c r="C2" s="11"/>
       <c r="D2">
         <v>58</v>
       </c>
@@ -9164,8 +9868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB755405-B760-4A9E-837E-B2DADF10CD2C}">
   <dimension ref="A1:M62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E79" sqref="E79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9173,8 +9877,8 @@
     <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.21875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
@@ -9184,53 +9888,53 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" t="s">
         <v>40</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>41</v>
       </c>
-      <c r="C1" t="s">
-        <v>42</v>
-      </c>
       <c r="D1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" t="s">
         <v>46</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
+        <v>211</v>
+      </c>
+      <c r="G1" t="s">
+        <v>208</v>
+      </c>
+      <c r="H1" t="s">
         <v>47</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>212</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>209</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>48</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>213</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>210</v>
-      </c>
-      <c r="K1" t="s">
-        <v>49</v>
-      </c>
-      <c r="L1" t="s">
-        <v>214</v>
-      </c>
-      <c r="M1" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="B2" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="C2" s="10"/>
+      <c r="C2" s="11"/>
       <c r="D2">
         <v>58</v>
       </c>
@@ -9754,29 +10458,38 @@
         <v>0.26223917082703202</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
+        <v>221</v>
+      </c>
+      <c r="B21" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>222</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" t="s">
+        <v>225</v>
+      </c>
+      <c r="C22" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>223</v>
-      </c>
-      <c r="B22" t="s">
+      <c r="D22" t="s">
         <v>226</v>
       </c>
-      <c r="C22" t="s">
-        <v>225</v>
-      </c>
-      <c r="D22" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E22" t="s">
+        <v>48</v>
+      </c>
+      <c r="F22" t="s">
+        <v>213</v>
+      </c>
+      <c r="G22" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>8</v>
       </c>
@@ -9789,8 +10502,17 @@
       <c r="D23" s="5">
         <v>1.85</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E23" s="5">
+        <v>0.42333568543663103</v>
+      </c>
+      <c r="F23" s="5">
+        <v>0.29399999999999998</v>
+      </c>
+      <c r="G23" s="5">
+        <v>0.267695004407283</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>16</v>
       </c>
@@ -9803,8 +10525,17 @@
       <c r="D24" s="5">
         <v>2.6829268292682902</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E24" s="5">
+        <v>0.39027640108581602</v>
+      </c>
+      <c r="F24" s="5">
+        <v>0.324756660834989</v>
+      </c>
+      <c r="G24" s="5">
+        <v>0.268942273472282</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -9817,8 +10548,17 @@
       <c r="D25" s="5">
         <v>3.2857142857142798</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E25" s="5">
+        <v>0.32426568627302699</v>
+      </c>
+      <c r="F25" s="5">
+        <v>0.30430944003451099</v>
+      </c>
+      <c r="G25" s="5">
+        <v>0.317074865904308</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>32</v>
       </c>
@@ -9831,8 +10571,17 @@
       <c r="D26" s="5">
         <v>3.7105263157894699</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E26" s="5">
+        <v>0.27187430871537299</v>
+      </c>
+      <c r="F26" s="5">
+        <v>0.22306152136773999</v>
+      </c>
+      <c r="G26" s="5">
+        <v>0.23268538219111001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>40</v>
       </c>
@@ -9845,27 +10594,45 @@
       <c r="D27" s="5">
         <v>4.1219512195121899</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E27" s="5">
+        <v>0.209743051210836</v>
+      </c>
+      <c r="F27" s="5">
+        <v>0.122812955386261</v>
+      </c>
+      <c r="G27" s="5">
+        <v>0.20755246321142001</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>229</v>
-      </c>
       <c r="B42" t="s">
+        <v>225</v>
+      </c>
+      <c r="C42" t="s">
+        <v>224</v>
+      </c>
+      <c r="D42" t="s">
         <v>226</v>
       </c>
-      <c r="C42" t="s">
-        <v>225</v>
-      </c>
-      <c r="D42" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E42" t="s">
+        <v>48</v>
+      </c>
+      <c r="F42" t="s">
+        <v>213</v>
+      </c>
+      <c r="G42" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>0</v>
       </c>
@@ -9878,8 +10645,17 @@
       <c r="D43" s="5">
         <v>1.875</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E43" s="5">
+        <v>0.28764935919649398</v>
+      </c>
+      <c r="F43" s="5">
+        <v>0.413998141950494</v>
+      </c>
+      <c r="G43" s="5">
+        <v>0.28235706617776102</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>10</v>
       </c>
@@ -9892,8 +10668,17 @@
       <c r="D44" s="5">
         <v>2.5128205128205101</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E44" s="5">
+        <v>0.36350287997334801</v>
+      </c>
+      <c r="F44" s="5">
+        <v>0.29440044472695198</v>
+      </c>
+      <c r="G44" s="5">
+        <v>0.32097079291555602</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>20</v>
       </c>
@@ -9906,8 +10691,17 @@
       <c r="D45" s="5">
         <v>3.1590909090908998</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E45" s="5">
+        <v>0.28140240761331597</v>
+      </c>
+      <c r="F45" s="5">
+        <v>0.31476409685850598</v>
+      </c>
+      <c r="G45" s="5">
+        <v>0.26230585747858598</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>30</v>
       </c>
@@ -9920,8 +10714,17 @@
       <c r="D46" s="5">
         <v>3.375</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E46" s="5">
+        <v>0.25677841390224698</v>
+      </c>
+      <c r="F46" s="5">
+        <v>0.262117413503068</v>
+      </c>
+      <c r="G46" s="5">
+        <v>0.206850311293097</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>40</v>
       </c>
@@ -9934,29 +10737,47 @@
       <c r="D47" s="5">
         <v>4.1219512195121899</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E47" s="5">
+        <v>0.209743051210836</v>
+      </c>
+      <c r="F47" s="5">
+        <v>0.122812955386261</v>
+      </c>
+      <c r="G47" s="5">
+        <v>0.20755246321142001</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
+      <c r="B58" t="s">
+        <v>225</v>
+      </c>
+      <c r="C58" t="s">
+        <v>224</v>
+      </c>
+      <c r="D58" t="s">
+        <v>226</v>
+      </c>
+      <c r="E58" t="s">
+        <v>48</v>
+      </c>
+      <c r="F58" t="s">
+        <v>213</v>
+      </c>
+      <c r="G58" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A59" s="8" t="s">
         <v>231</v>
-      </c>
-      <c r="B58" t="s">
-        <v>226</v>
-      </c>
-      <c r="C58" t="s">
-        <v>225</v>
-      </c>
-      <c r="D58" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A59" s="8" t="s">
-        <v>232</v>
       </c>
       <c r="B59" s="5">
         <v>1.8571428571428501</v>
@@ -9967,10 +10788,19 @@
       <c r="D59" s="5">
         <v>2.02857142857142</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E59" s="5">
+        <v>0.37810673874231898</v>
+      </c>
+      <c r="F59" s="5">
+        <v>0.35469556125848301</v>
+      </c>
+      <c r="G59" s="5">
+        <v>0.295076460679361</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" s="9" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B60" s="5">
         <v>2.1714285714285699</v>
@@ -9981,10 +10811,19 @@
       <c r="D60" s="5">
         <v>2.6</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E60" s="5">
+        <v>0.28392542517151098</v>
+      </c>
+      <c r="F60" s="5">
+        <v>0.34413677171592499</v>
+      </c>
+      <c r="G60" s="5">
+        <v>0.256624238917527</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" s="9" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B61" s="5">
         <v>3</v>
@@ -9995,10 +10834,19 @@
       <c r="D61" s="5">
         <v>3.38888888888888</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E61" s="5">
+        <v>0.29217954905997201</v>
+      </c>
+      <c r="F61" s="5">
+        <v>0.30743382305067701</v>
+      </c>
+      <c r="G61" s="5">
+        <v>0.26223917082703202</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="9" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B62" s="5">
         <v>3.9268292682926802</v>
@@ -10008,6 +10856,15 @@
       </c>
       <c r="D62" s="5">
         <v>4.1219512195121899</v>
+      </c>
+      <c r="E62" s="5">
+        <v>0.209743051210836</v>
+      </c>
+      <c r="F62" s="5">
+        <v>0.122812955386261</v>
+      </c>
+      <c r="G62" s="5">
+        <v>0.20755246321142001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
static on presentation order
</commit_message>
<xml_diff>
--- a/p835_reference_conditions/CSP835_Ref_Conditions.xlsx
+++ b/p835_reference_conditions/CSP835_Ref_Conditions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\hitapp\P.835\p835_reference_conditions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC7896C5-47DB-450B-8C0A-4BD02A8879FC}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4033EAC4-42E0-4B5F-84A6-86FAB6764108}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="12855" firstSheet="1" activeTab="3" xr2:uid="{26D8FBFA-0696-4DB3-897E-8243390CDEAA}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="12852" firstSheet="1" activeTab="5" xr2:uid="{26D8FBFA-0696-4DB3-897E-8243390CDEAA}"/>
   </bookViews>
   <sheets>
     <sheet name="description" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="248">
   <si>
     <t>c1</t>
   </si>
@@ -761,6 +761,21 @@
   </si>
   <si>
     <t>degraded_WB_16KHz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Yi Hu and Philipos C. Loizou 2007 </t>
+  </si>
+  <si>
+    <t>correlation</t>
+  </si>
+  <si>
+    <t>RMSE</t>
+  </si>
+  <si>
+    <t>diff</t>
+  </si>
+  <si>
+    <t>Predicted MOS_OVRL from SIG and BAK (accoirdomg to [1])</t>
   </si>
 </sst>
 </file>
@@ -9821,12 +9836,12 @@
       <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.53125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -9834,7 +9849,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -9842,7 +9857,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -9850,7 +9865,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -9858,16 +9873,16 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -9875,7 +9890,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -9883,7 +9898,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -9891,7 +9906,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -9899,7 +9914,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -9907,7 +9922,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>35</v>
       </c>
@@ -9915,7 +9930,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -9923,7 +9938,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -9931,7 +9946,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -9939,13 +9954,13 @@
         <v>220</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B17" s="2"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -9953,7 +9968,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>29</v>
       </c>
@@ -9961,7 +9976,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>235</v>
       </c>
@@ -9969,13 +9984,13 @@
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>241</v>
       </c>
       <c r="B21" s="2"/>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>236</v>
       </c>
@@ -9983,7 +9998,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
         <v>238</v>
       </c>
@@ -9991,13 +10006,13 @@
         <v>214</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>242</v>
       </c>
       <c r="B24" s="2"/>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
         <v>236</v>
       </c>
@@ -10005,7 +10020,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="10" t="s">
         <v>238</v>
       </c>
@@ -10013,12 +10028,12 @@
         <v>240</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="33" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C33" s="7"/>
     </row>
   </sheetData>
@@ -10034,16 +10049,16 @@
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.46484375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.46484375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>38</v>
       </c>
@@ -10063,7 +10078,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -10081,7 +10096,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -10101,7 +10116,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -10121,7 +10136,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -10141,7 +10156,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -10161,7 +10176,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -10181,7 +10196,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -10201,7 +10216,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -10221,7 +10236,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -10241,7 +10256,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -10261,7 +10276,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -10281,7 +10296,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -10301,7 +10316,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -10337,21 +10352,21 @@
       <selection activeCell="D74" sqref="D74:D79"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="42.19921875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.46484375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.86328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.1328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.53125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.1328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="10.53125" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="12.1328125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.53125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>44</v>
       </c>
@@ -10392,7 +10407,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>51</v>
       </c>
@@ -10433,7 +10448,7 @@
         <v>0.33850349390311302</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>53</v>
       </c>
@@ -10474,7 +10489,7 @@
         <v>0.47811198937086402</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>55</v>
       </c>
@@ -10515,7 +10530,7 @@
         <v>0.27999999999999903</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>57</v>
       </c>
@@ -10556,7 +10571,7 @@
         <v>0.368529702214273</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>59</v>
       </c>
@@ -10597,7 +10612,7 @@
         <v>0.41320428092866801</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>61</v>
       </c>
@@ -10638,7 +10653,7 @@
         <v>0.244999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>63</v>
       </c>
@@ -10679,7 +10694,7 @@
         <v>0.48009998958550199</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>65</v>
       </c>
@@ -10720,7 +10735,7 @@
         <v>0.66653331999733201</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>67</v>
       </c>
@@ -10761,7 +10776,7 @@
         <v>0.786717512481096</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>69</v>
       </c>
@@ -10802,7 +10817,7 @@
         <v>0.41320428092866801</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>71</v>
       </c>
@@ -10843,7 +10858,7 @@
         <v>0.37040518354904201</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>73</v>
       </c>
@@ -10884,7 +10899,7 @@
         <v>0.82825116963394596</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>111</v>
       </c>
@@ -10925,7 +10940,7 @@
         <v>1.14286657138967</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>113</v>
       </c>
@@ -10966,7 +10981,7 @@
         <v>0.58286647985051698</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>115</v>
       </c>
@@ -11007,7 +11022,7 @@
         <v>0.58286647985051698</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>117</v>
       </c>
@@ -11048,7 +11063,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>119</v>
       </c>
@@ -11089,7 +11104,7 @@
         <v>0.63484250015259602</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>121</v>
       </c>
@@ -11130,7 +11145,7 @@
         <v>0.74081036709808501</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>123</v>
       </c>
@@ -11171,7 +11186,7 @@
         <v>0.98</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>125</v>
       </c>
@@ -11212,7 +11227,7 @@
         <v>0.99940782466418498</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>127</v>
       </c>
@@ -11253,7 +11268,7 @@
         <v>0.93543097613405501</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>129</v>
       </c>
@@ -11294,7 +11309,7 @@
         <v>0.41320428092866801</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>131</v>
       </c>
@@ -11335,7 +11350,7 @@
         <v>0.65333333333333299</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>133</v>
       </c>
@@ -11376,7 +11391,7 @@
         <v>0.506069823904435</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>135</v>
       </c>
@@ -11417,7 +11432,7 @@
         <v>0.60234357120980198</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>137</v>
       </c>
@@ -11458,7 +11473,7 @@
         <v>0.41320428092866801</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>139</v>
       </c>
@@ -11499,7 +11514,7 @@
         <v>0.41320428092866801</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>141</v>
       </c>
@@ -11540,7 +11555,7 @@
         <v>0.515582195192968</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>143</v>
       </c>
@@ -11581,7 +11596,7 @@
         <v>0.786717512481096</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>145</v>
       </c>
@@ -11622,7 +11637,7 @@
         <v>0.506069823904435</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>147</v>
       </c>
@@ -11663,7 +11678,7 @@
         <v>0.60234357120980198</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>149</v>
       </c>
@@ -11704,7 +11719,7 @@
         <v>0.39597979746446599</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>151</v>
       </c>
@@ -11745,7 +11760,7 @@
         <v>0.43826932358995802</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>153</v>
       </c>
@@ -11786,7 +11801,7 @@
         <v>0.65333333333333299</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>155</v>
       </c>
@@ -11827,7 +11842,7 @@
         <v>0.244999999999999</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>157</v>
       </c>
@@ -11868,7 +11883,7 @@
         <v>0.48999999999999899</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>159</v>
       </c>
@@ -11909,7 +11924,7 @@
         <v>0.74081036709808501</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>161</v>
       </c>
@@ -11950,7 +11965,7 @@
         <v>0.65333333333333299</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>163</v>
       </c>
@@ -11991,7 +12006,7 @@
         <v>0.65333333333333299</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>165</v>
       </c>
@@ -12032,7 +12047,7 @@
         <v>0.78027238833627799</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>167</v>
       </c>
@@ -12073,7 +12088,7 @@
         <v>0.65333333333333299</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>169</v>
       </c>
@@ -12114,7 +12129,7 @@
         <v>0.65333333333333299</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>171</v>
       </c>
@@ -12155,7 +12170,7 @@
         <v>0.93543097613405501</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>173</v>
       </c>
@@ -12196,7 +12211,7 @@
         <v>0.82429768085726496</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>175</v>
       </c>
@@ -12237,7 +12252,7 @@
         <v>0.786717512481096</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>177</v>
       </c>
@@ -12278,7 +12293,7 @@
         <v>0.786717512481096</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>179</v>
       </c>
@@ -12319,7 +12334,7 @@
         <v>0.60234357120980198</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>181</v>
       </c>
@@ -12360,7 +12375,7 @@
         <v>0.61424750711744802</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>183</v>
       </c>
@@ -12401,7 +12416,7 @@
         <v>0.506069823904435</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>185</v>
       </c>
@@ -12442,7 +12457,7 @@
         <v>0.61424750711744802</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>187</v>
       </c>
@@ -12483,7 +12498,7 @@
         <v>0.71728655361717097</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>189</v>
       </c>
@@ -12524,7 +12539,7 @@
         <v>0.78027238833627799</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>191</v>
       </c>
@@ -12565,7 +12580,7 @@
         <v>0.61424750711744802</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>193</v>
       </c>
@@ -12606,7 +12621,7 @@
         <v>0.71569080847341704</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>195</v>
       </c>
@@ -12647,7 +12662,7 @@
         <v>0.36147844564602499</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>197</v>
       </c>
@@ -12688,7 +12703,7 @@
         <v>0.42770706486254501</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>199</v>
       </c>
@@ -12729,7 +12744,7 @@
         <v>0.41320428092866801</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>201</v>
       </c>
@@ -12770,7 +12785,7 @@
         <v>0.66946745004269304</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>203</v>
       </c>
@@ -12811,7 +12826,7 @@
         <v>0.63484250015259602</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>205</v>
       </c>
@@ -12852,7 +12867,7 @@
         <v>0.43826932358995802</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>75</v>
       </c>
@@ -12893,7 +12908,7 @@
         <v>0.60234357120980198</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>77</v>
       </c>
@@ -12934,7 +12949,7 @@
         <v>0.48009998958550199</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>79</v>
       </c>
@@ -12975,7 +12990,7 @@
         <v>0.96904993564716602</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>81</v>
       </c>
@@ -13016,7 +13031,7 @@
         <v>0.71569080847341704</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>83</v>
       </c>
@@ -13057,7 +13072,7 @@
         <v>0.786717512481096</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>85</v>
       </c>
@@ -13098,7 +13113,7 @@
         <v>0.786717512481096</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>87</v>
       </c>
@@ -13139,7 +13154,7 @@
         <v>0.99940782466418498</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>89</v>
       </c>
@@ -13180,7 +13195,7 @@
         <v>0.99940782466418498</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>91</v>
       </c>
@@ -13221,7 +13236,7 @@
         <v>0.58286647985051698</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>93</v>
       </c>
@@ -13262,7 +13277,7 @@
         <v>0.506069823904435</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>95</v>
       </c>
@@ -13303,7 +13318,7 @@
         <v>0.43826932358995802</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>97</v>
       </c>
@@ -13344,7 +13359,7 @@
         <v>0.43826932358995802</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>99</v>
       </c>
@@ -13385,7 +13400,7 @@
         <v>0.82640856185733602</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>101</v>
       </c>
@@ -13426,7 +13441,7 @@
         <v>0.66946745004269304</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>103</v>
       </c>
@@ -13467,7 +13482,7 @@
         <v>0.41320428092866801</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>105</v>
       </c>
@@ -13508,7 +13523,7 @@
         <v>0.61980642139300202</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>107</v>
       </c>
@@ -13549,7 +13564,7 @@
         <v>0.99940782466418498</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>109</v>
       </c>
@@ -13600,20 +13615,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60F8B73C-7BC7-4826-AE79-6F2DE370CA9C}">
   <dimension ref="A1:M79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:M79"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="Q25" sqref="Q25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="42.19921875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.46484375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.86328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="13" width="13.265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="13" width="13.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>44</v>
       </c>
@@ -13654,7 +13669,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>51</v>
       </c>
@@ -13695,7 +13710,7 @@
         <v>0.32385456269408602</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>53</v>
       </c>
@@ -13736,7 +13751,7 @@
         <v>0.27858226937133002</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>55</v>
       </c>
@@ -13777,7 +13792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>57</v>
       </c>
@@ -13818,7 +13833,7 @@
         <v>0.275265695566698</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>59</v>
       </c>
@@ -13859,7 +13874,7 @@
         <v>0.35864327680858499</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>61</v>
       </c>
@@ -13900,7 +13915,7 @@
         <v>0.288092920538144</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>63</v>
       </c>
@@ -13941,7 +13956,7 @@
         <v>0.41320428092866801</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>65</v>
       </c>
@@ -13982,7 +13997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>67</v>
       </c>
@@ -14023,7 +14038,7 @@
         <v>0.60234357120980198</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>69</v>
       </c>
@@ -14064,7 +14079,7 @@
         <v>0.64156059729381698</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>71</v>
       </c>
@@ -14105,7 +14120,7 @@
         <v>0.34433690077389001</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>73</v>
       </c>
@@ -14146,7 +14161,7 @@
         <v>0.51120772033815498</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>111</v>
       </c>
@@ -14187,7 +14202,7 @@
         <v>0.41320428092866801</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>113</v>
       </c>
@@ -14228,7 +14243,7 @@
         <v>0.60234357120980198</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>115</v>
       </c>
@@ -14269,7 +14284,7 @@
         <v>0.41320428092866801</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>117</v>
       </c>
@@ -14310,7 +14325,7 @@
         <v>0.48999999999999899</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>119</v>
       </c>
@@ -14351,7 +14366,7 @@
         <v>0.54444444444444395</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>121</v>
       </c>
@@ -14392,7 +14407,7 @@
         <v>0.60486913185140001</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>123</v>
       </c>
@@ -14433,7 +14448,7 @@
         <v>0.44410021391573301</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>125</v>
       </c>
@@ -14474,7 +14489,7 @@
         <v>0.60234357120980198</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>127</v>
       </c>
@@ -14515,7 +14530,7 @@
         <v>0.32666666666666599</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>129</v>
       </c>
@@ -14556,7 +14571,7 @@
         <v>0.41320428092866801</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>131</v>
       </c>
@@ -14597,7 +14612,7 @@
         <v>0.83922186180612102</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>133</v>
       </c>
@@ -14638,7 +14653,7 @@
         <v>0.41320428092866801</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>135</v>
       </c>
@@ -14679,7 +14694,7 @@
         <v>0.44410021391573301</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>137</v>
       </c>
@@ -14720,7 +14735,7 @@
         <v>0.60234357120980198</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>139</v>
       </c>
@@ -14761,7 +14776,7 @@
         <v>0.37040518354904201</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>141</v>
       </c>
@@ -14802,7 +14817,7 @@
         <v>0.56580326380583301</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>143</v>
       </c>
@@ -14843,7 +14858,7 @@
         <v>0.51120772033815498</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>145</v>
       </c>
@@ -14884,7 +14899,7 @@
         <v>0.32666666666666599</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>147</v>
       </c>
@@ -14925,7 +14940,7 @@
         <v>0.32078029864690799</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>149</v>
       </c>
@@ -14966,7 +14981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>151</v>
       </c>
@@ -15007,7 +15022,7 @@
         <v>0.506069823904435</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>153</v>
       </c>
@@ -15048,7 +15063,7 @@
         <v>0.35864327680858499</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>155</v>
       </c>
@@ -15089,7 +15104,7 @@
         <v>0.39260447221718903</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>157</v>
       </c>
@@ -15130,7 +15145,7 @@
         <v>0.43555555555555497</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>159</v>
       </c>
@@ -15171,7 +15186,7 @@
         <v>0.86427876161443196</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>161</v>
       </c>
@@ -15212,7 +15227,7 @@
         <v>1.0844353369380699</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>163</v>
       </c>
@@ -15253,7 +15268,7 @@
         <v>1.0844353369380699</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>165</v>
       </c>
@@ -15294,7 +15309,7 @@
         <v>1.02241544067631</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>167</v>
       </c>
@@ -15335,7 +15350,7 @@
         <v>0.786717512481096</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>169</v>
       </c>
@@ -15376,7 +15391,7 @@
         <v>0.786717512481096</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>171</v>
       </c>
@@ -15417,7 +15432,7 @@
         <v>0.37040518354904201</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>173</v>
       </c>
@@ -15458,7 +15473,7 @@
         <v>0.506069823904435</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>175</v>
       </c>
@@ -15499,7 +15514,7 @@
         <v>0.61424750711744802</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>177</v>
       </c>
@@ -15540,7 +15555,7 @@
         <v>0.82429768085726496</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>179</v>
       </c>
@@ -15581,7 +15596,7 @@
         <v>0.900074071026009</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>181</v>
       </c>
@@ -15622,7 +15637,7 @@
         <v>0.79195959492893298</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>183</v>
       </c>
@@ -15663,7 +15678,7 @@
         <v>0.87653864717991703</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>185</v>
       </c>
@@ -15704,7 +15719,7 @@
         <v>0.76222222222222202</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>187</v>
       </c>
@@ -15745,7 +15760,7 @@
         <v>0.58286647985051698</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>189</v>
       </c>
@@ -15786,7 +15801,7 @@
         <v>0.72295689129205098</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>191</v>
       </c>
@@ -15827,7 +15842,7 @@
         <v>0.55999999999999905</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>193</v>
       </c>
@@ -15868,7 +15883,7 @@
         <v>0.41320428092866801</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>195</v>
       </c>
@@ -15909,7 +15924,7 @@
         <v>0.41320428092866801</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>197</v>
       </c>
@@ -15950,7 +15965,7 @@
         <v>0.506069823904435</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>199</v>
       </c>
@@ -15991,7 +16006,7 @@
         <v>0.66946745004269304</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>201</v>
       </c>
@@ -16032,7 +16047,7 @@
         <v>0.55999999999999905</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>203</v>
       </c>
@@ -16073,7 +16088,7 @@
         <v>0.51120772033815498</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>205</v>
       </c>
@@ -16114,7 +16129,7 @@
         <v>0.66946745004269304</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>75</v>
       </c>
@@ -16155,7 +16170,7 @@
         <v>0.244999999999999</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>77</v>
       </c>
@@ -16196,7 +16211,7 @@
         <v>0.93543097613405501</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>79</v>
       </c>
@@ -16237,7 +16252,7 @@
         <v>0.96904993564716602</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>81</v>
       </c>
@@ -16278,7 +16293,7 @@
         <v>0.63484250015259602</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>83</v>
       </c>
@@ -16319,7 +16334,7 @@
         <v>1.03511674059821</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>85</v>
       </c>
@@ -16360,7 +16375,7 @@
         <v>0.60486913185140001</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>87</v>
       </c>
@@ -16401,7 +16416,7 @@
         <v>0.506069823904435</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>89</v>
       </c>
@@ -16442,7 +16457,7 @@
         <v>0.66946745004269304</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>91</v>
       </c>
@@ -16483,7 +16498,7 @@
         <v>0.786717512481096</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>93</v>
       </c>
@@ -16524,7 +16539,7 @@
         <v>0.786717512481096</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>95</v>
       </c>
@@ -16565,7 +16580,7 @@
         <v>0.48999999999999899</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>97</v>
       </c>
@@ -16606,7 +16621,7 @@
         <v>0.32078029864690799</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>99</v>
       </c>
@@ -16647,7 +16662,7 @@
         <v>0.32078029864690799</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>101</v>
       </c>
@@ -16688,7 +16703,7 @@
         <v>0.37040518354904201</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>103</v>
       </c>
@@ -16729,7 +16744,7 @@
         <v>0.44410021391573301</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>105</v>
       </c>
@@ -16770,7 +16785,7 @@
         <v>0.66946745004269304</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>107</v>
       </c>
@@ -16811,7 +16826,7 @@
         <v>0.66946745004269304</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>109</v>
       </c>
@@ -16866,21 +16881,21 @@
       <selection activeCell="D2" sqref="D2:D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.46484375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.1328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.53125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.19921875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.19921875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>39</v>
       </c>
@@ -16921,7 +16936,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>42</v>
       </c>
@@ -16960,7 +16975,7 @@
         <v>0.16144674678505899</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -17001,7 +17016,7 @@
         <v>0.267695004407283</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -17042,7 +17057,7 @@
         <v>0.268942273472282</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -17083,7 +17098,7 @@
         <v>0.317074865904308</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -17124,7 +17139,7 @@
         <v>0.23268538219111001</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -17165,7 +17180,7 @@
         <v>0.20755246321142001</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -17206,7 +17221,7 @@
         <v>0.28235706617776102</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -17247,7 +17262,7 @@
         <v>0.32097079291555602</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -17288,7 +17303,7 @@
         <v>0.26230585747858598</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -17329,7 +17344,7 @@
         <v>0.206850311293097</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -17370,7 +17385,7 @@
         <v>0.295076460679361</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -17411,7 +17426,7 @@
         <v>0.256624238917527</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -17462,27 +17477,27 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A93CA3CB-7667-4296-BFB2-B367E47E0614}">
-  <dimension ref="A1:M15"/>
+  <dimension ref="A1:T17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.46484375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.1328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.53125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.19921875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.19921875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>39</v>
       </c>
@@ -17522,8 +17537,14 @@
       <c r="M1" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="P1" t="s">
+        <v>247</v>
+      </c>
+      <c r="T1" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>42</v>
       </c>
@@ -17561,8 +17582,16 @@
       <c r="M2" s="5">
         <v>0.12668238599562701</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="P2">
+        <f>-0.0783+0.571*F2+0.366*E2</f>
+        <v>4.3791920634920602</v>
+      </c>
+      <c r="T2" s="5">
+        <f>G2-P2</f>
+        <v>0.27160158730159001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -17602,8 +17631,23 @@
       <c r="M3" s="5">
         <v>0.199859028908664</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="P3">
+        <f t="shared" ref="P3:P14" si="0">-0.0783+0.571*F3+0.366*E3</f>
+        <v>2.0867476190476157</v>
+      </c>
+      <c r="R3" t="s">
+        <v>244</v>
+      </c>
+      <c r="S3">
+        <f>CORREL(G2:G14,P2:P14)</f>
+        <v>0.98284834913620556</v>
+      </c>
+      <c r="T3" s="5">
+        <f t="shared" ref="T3:T14" si="1">G3-P3</f>
+        <v>-0.13436666666666564</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -17643,8 +17687,23 @@
       <c r="M4" s="5">
         <v>0.213356197961699</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="P4">
+        <f t="shared" si="0"/>
+        <v>2.8759619047618976</v>
+      </c>
+      <c r="R4" t="s">
+        <v>245</v>
+      </c>
+      <c r="S4">
+        <f>SQRT(SUMSQ(T2:T14)/COUNTA(T2:T14))</f>
+        <v>0.19955813133179501</v>
+      </c>
+      <c r="T4" s="5">
+        <f t="shared" si="1"/>
+        <v>4.9904761904824291E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -17684,8 +17743,16 @@
       <c r="M5" s="5">
         <v>0.217181852088391</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="P5">
+        <f t="shared" si="0"/>
+        <v>3.4886210526315722</v>
+      </c>
+      <c r="T5" s="5">
+        <f t="shared" si="1"/>
+        <v>9.0326315789477807E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -17725,8 +17792,16 @@
       <c r="M6" s="5">
         <v>0.20514766881347701</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="P6">
+        <f t="shared" si="0"/>
+        <v>3.6514045454545423</v>
+      </c>
+      <c r="T6" s="5">
+        <f t="shared" si="1"/>
+        <v>7.5868181818177671E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -17766,8 +17841,16 @@
       <c r="M7" s="5">
         <v>0.15296989886932699</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="P7">
+        <f t="shared" si="0"/>
+        <v>3.7276347826086913</v>
+      </c>
+      <c r="T7" s="5">
+        <f t="shared" si="1"/>
+        <v>9.8452173913038621E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -17807,8 +17890,16 @@
       <c r="M8" s="5">
         <v>0.37482425872967301</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="P8">
+        <f t="shared" si="0"/>
+        <v>2.348938095238092</v>
+      </c>
+      <c r="T8" s="5">
+        <f t="shared" si="1"/>
+        <v>-0.37274761904762199</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -17848,8 +17939,16 @@
       <c r="M9" s="5">
         <v>0.27939361054972001</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="P9">
+        <f t="shared" si="0"/>
+        <v>2.9159093023255798</v>
+      </c>
+      <c r="T9" s="5">
+        <f t="shared" si="1"/>
+        <v>-0.45079302325581994</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -17889,8 +17988,16 @@
       <c r="M10" s="5">
         <v>0.27269606456902901</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="P10">
+        <f t="shared" si="0"/>
+        <v>3.204366666666659</v>
+      </c>
+      <c r="T10" s="5">
+        <f t="shared" si="1"/>
+        <v>0.12896666666667089</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -17930,8 +18037,16 @@
       <c r="M11" s="5">
         <v>0.230823869229277</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="P11">
+        <f t="shared" si="0"/>
+        <v>3.6115421052631502</v>
+      </c>
+      <c r="T11" s="5">
+        <f t="shared" si="1"/>
+        <v>-0.11154210526315023</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -17971,8 +18086,16 @@
       <c r="M12" s="5">
         <v>0.298367736581994</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="P12">
+        <f t="shared" si="0"/>
+        <v>2.5270571428571382</v>
+      </c>
+      <c r="T12" s="5">
+        <f t="shared" si="1"/>
+        <v>-0.14610476190475818</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -18012,8 +18135,16 @@
       <c r="M13" s="5">
         <v>0.23786006444212099</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="P13">
+        <f t="shared" si="0"/>
+        <v>3.1126499999999999</v>
+      </c>
+      <c r="T13" s="5">
+        <f t="shared" si="1"/>
+        <v>-8.7650000000000006E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -18053,8 +18184,16 @@
       <c r="M14" s="5">
         <v>0.20088853133069001</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="P14">
+        <f t="shared" si="0"/>
+        <v>3.2220333333333295</v>
+      </c>
+      <c r="T14" s="5">
+        <f t="shared" si="1"/>
+        <v>4.4633333333330416E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
@@ -18064,6 +18203,11 @@
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
       <c r="M15" s="5"/>
+    </row>
+    <row r="17" spans="16:16" x14ac:dyDescent="0.3">
+      <c r="P17" t="s">
+        <v>243</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -18081,21 +18225,21 @@
       <selection activeCell="E79" sqref="E79"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.86328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.46484375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.19921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.21875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.19921875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.19921875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>39</v>
       </c>
@@ -18136,7 +18280,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>42</v>
       </c>
@@ -18175,7 +18319,7 @@
         <v>0.16144674678505899</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -18216,7 +18360,7 @@
         <v>0.267695004407283</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -18257,7 +18401,7 @@
         <v>0.268942273472282</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -18298,7 +18442,7 @@
         <v>0.317074865904308</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -18339,7 +18483,7 @@
         <v>0.23268538219111001</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -18380,7 +18524,7 @@
         <v>0.20755246321142001</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -18421,7 +18565,7 @@
         <v>0.28235706617776102</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -18462,7 +18606,7 @@
         <v>0.32097079291555602</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -18503,7 +18647,7 @@
         <v>0.26230585747858598</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -18544,7 +18688,7 @@
         <v>0.206850311293097</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -18585,7 +18729,7 @@
         <v>0.295076460679361</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -18626,7 +18770,7 @@
         <v>0.256624238917527</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -18667,7 +18811,7 @@
         <v>0.26223917082703202</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>221</v>
       </c>
@@ -18675,7 +18819,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>222</v>
       </c>
@@ -18698,7 +18842,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>8</v>
       </c>
@@ -18721,7 +18865,7 @@
         <v>0.267695004407283</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>16</v>
       </c>
@@ -18744,7 +18888,7 @@
         <v>0.268942273472282</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -18767,7 +18911,7 @@
         <v>0.317074865904308</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>32</v>
       </c>
@@ -18790,7 +18934,7 @@
         <v>0.23268538219111001</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>40</v>
       </c>
@@ -18813,12 +18957,12 @@
         <v>0.20755246321142001</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>228</v>
       </c>
@@ -18841,7 +18985,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>0</v>
       </c>
@@ -18864,7 +19008,7 @@
         <v>0.28235706617776102</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>10</v>
       </c>
@@ -18887,7 +19031,7 @@
         <v>0.32097079291555602</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>20</v>
       </c>
@@ -18910,7 +19054,7 @@
         <v>0.26230585747858598</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>30</v>
       </c>
@@ -18933,7 +19077,7 @@
         <v>0.206850311293097</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>40</v>
       </c>
@@ -18956,12 +19100,12 @@
         <v>0.20755246321142001</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>230</v>
       </c>
@@ -18984,7 +19128,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" s="8" t="s">
         <v>231</v>
       </c>
@@ -19007,7 +19151,7 @@
         <v>0.295076460679361</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" s="9" t="s">
         <v>232</v>
       </c>
@@ -19030,7 +19174,7 @@
         <v>0.256624238917527</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" s="9" t="s">
         <v>233</v>
       </c>
@@ -19053,7 +19197,7 @@
         <v>0.26223917082703202</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="9" t="s">
         <v>234</v>
       </c>
@@ -19093,21 +19237,21 @@
       <selection activeCell="G69" sqref="G69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.86328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.46484375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.19921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.21875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.19921875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.19921875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>39</v>
       </c>
@@ -19148,7 +19292,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>42</v>
       </c>
@@ -19187,7 +19331,7 @@
         <v>0.12668238599562701</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -19228,7 +19372,7 @@
         <v>0.199859028908664</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -19269,7 +19413,7 @@
         <v>0.213356197961699</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -19310,7 +19454,7 @@
         <v>0.217181852088391</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -19351,7 +19495,7 @@
         <v>0.20514766881347701</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -19392,7 +19536,7 @@
         <v>0.15296989886932699</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -19433,7 +19577,7 @@
         <v>0.37482425872967301</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -19474,7 +19618,7 @@
         <v>0.27939361054972001</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -19515,7 +19659,7 @@
         <v>0.27269606456902901</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -19556,7 +19700,7 @@
         <v>0.230823869229277</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -19597,7 +19741,7 @@
         <v>0.298367736581994</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -19638,7 +19782,7 @@
         <v>0.23786006444212099</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -19679,7 +19823,7 @@
         <v>0.20088853133069001</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>221</v>
       </c>
@@ -19687,7 +19831,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>222</v>
       </c>
@@ -19710,7 +19854,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>8</v>
       </c>
@@ -19733,7 +19877,7 @@
         <v>0.199859028908664</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>16</v>
       </c>
@@ -19756,7 +19900,7 @@
         <v>0.213356197961699</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -19779,7 +19923,7 @@
         <v>0.217181852088391</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>32</v>
       </c>
@@ -19802,7 +19946,7 @@
         <v>0.20514766881347701</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>40</v>
       </c>
@@ -19825,12 +19969,12 @@
         <v>0.15296989886932699</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>228</v>
       </c>
@@ -19853,7 +19997,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>0</v>
       </c>
@@ -19876,7 +20020,7 @@
         <v>0.37482425872967301</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>10</v>
       </c>
@@ -19899,7 +20043,7 @@
         <v>0.27939361054972001</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>20</v>
       </c>
@@ -19922,7 +20066,7 @@
         <v>0.27269606456902901</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>30</v>
       </c>
@@ -19945,7 +20089,7 @@
         <v>0.230823869229277</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>40</v>
       </c>
@@ -19968,12 +20112,12 @@
         <v>0.15296989886932699</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>230</v>
       </c>
@@ -19996,7 +20140,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" s="8" t="s">
         <v>231</v>
       </c>
@@ -20019,7 +20163,7 @@
         <v>0.298367736581994</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" s="9" t="s">
         <v>232</v>
       </c>
@@ -20042,7 +20186,7 @@
         <v>0.23786006444212099</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" s="9" t="s">
         <v>233</v>
       </c>
@@ -20065,7 +20209,7 @@
         <v>0.20088853133069001</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="9" t="s">
         <v>234</v>
       </c>

</xml_diff>

<commit_message>
goldclips will not add up in the aggregation
</commit_message>
<xml_diff>
--- a/p835_reference_conditions/CSP835_Ref_Conditions.xlsx
+++ b/p835_reference_conditions/CSP835_Ref_Conditions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\hitapp\P.835\p835_reference_conditions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4033EAC4-42E0-4B5F-84A6-86FAB6764108}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89878185-24B5-41A7-8F59-82C8A2488B7F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="12852" firstSheet="1" activeTab="5" xr2:uid="{26D8FBFA-0696-4DB3-897E-8243390CDEAA}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="12852" xr2:uid="{26D8FBFA-0696-4DB3-897E-8243390CDEAA}"/>
   </bookViews>
   <sheets>
     <sheet name="description" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="250">
   <si>
     <t>c1</t>
   </si>
@@ -739,9 +739,6 @@
     <t>40/40</t>
   </si>
   <si>
-    <t>references</t>
-  </si>
-  <si>
     <t>sample rate</t>
   </si>
   <si>
@@ -776,6 +773,15 @@
   </si>
   <si>
     <t>Predicted MOS_OVRL from SIG and BAK (accoirdomg to [1])</t>
+  </si>
+  <si>
+    <t>noise</t>
+  </si>
+  <si>
+    <t>white background noise</t>
+  </si>
+  <si>
+    <t>referenc condition</t>
   </si>
 </sst>
 </file>
@@ -9832,8 +9838,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EF8797D-78C9-4C44-9CB3-1E03D4B2359C}">
   <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9978,7 +9984,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>235</v>
+        <v>249</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>42</v>
@@ -9986,21 +9992,21 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B21" s="2"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
+        <v>235</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>236</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>214</v>
@@ -10008,24 +10014,32 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B24" s="2"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="10" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="B27" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
@@ -10072,10 +10086,10 @@
         <v>41</v>
       </c>
       <c r="E1" t="s">
+        <v>240</v>
+      </c>
+      <c r="F1" t="s">
         <v>241</v>
-      </c>
-      <c r="F1" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -10093,7 +10107,7 @@
         <v>214</v>
       </c>
       <c r="F2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -10113,7 +10127,7 @@
         <v>214</v>
       </c>
       <c r="F3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -10133,7 +10147,7 @@
         <v>214</v>
       </c>
       <c r="F4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -10153,7 +10167,7 @@
         <v>214</v>
       </c>
       <c r="F5" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -10173,7 +10187,7 @@
         <v>214</v>
       </c>
       <c r="F6" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -10193,7 +10207,7 @@
         <v>214</v>
       </c>
       <c r="F7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -10213,7 +10227,7 @@
         <v>214</v>
       </c>
       <c r="F8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -10233,7 +10247,7 @@
         <v>214</v>
       </c>
       <c r="F9" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -10253,7 +10267,7 @@
         <v>214</v>
       </c>
       <c r="F10" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -10273,7 +10287,7 @@
         <v>214</v>
       </c>
       <c r="F11" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -10293,7 +10307,7 @@
         <v>214</v>
       </c>
       <c r="F12" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -10313,7 +10327,7 @@
         <v>214</v>
       </c>
       <c r="F13" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -10333,7 +10347,7 @@
         <v>214</v>
       </c>
       <c r="F14" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
   </sheetData>
@@ -17479,7 +17493,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A93CA3CB-7667-4296-BFB2-B367E47E0614}">
   <dimension ref="A1:T17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
@@ -17538,10 +17552,10 @@
         <v>210</v>
       </c>
       <c r="P1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="T1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
@@ -17636,7 +17650,7 @@
         <v>2.0867476190476157</v>
       </c>
       <c r="R3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="S3">
         <f>CORREL(G2:G14,P2:P14)</f>
@@ -17692,7 +17706,7 @@
         <v>2.8759619047618976</v>
       </c>
       <c r="R4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="S4">
         <f>SQRT(SUMSQ(T2:T14)/COUNTA(T2:T14))</f>
@@ -18206,7 +18220,7 @@
     </row>
     <row r="17" spans="16:16" x14ac:dyDescent="0.3">
       <c r="P17" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
   </sheetData>

</xml_diff>